<commit_message>
missing 0s in guilds model
</commit_message>
<xml_diff>
--- a/outputs/Anova Arthropoda Guilds.xlsx
+++ b/outputs/Anova Arthropoda Guilds.xlsx
@@ -387,17 +387,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>F:(1, 114)345.5, 0</t>
+          <t>F:(1, 132)249.9, 0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F:(1, 97)382.3, 0</t>
+          <t>F:(1, 132)275.7, 0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>F:(1, 126)831.5, 0</t>
+          <t>F:(1, 193)322.8, 0</t>
         </is>
       </c>
     </row>
@@ -409,17 +409,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F:(2, 114)73.5, 0</t>
+          <t>F:(2, 132)105.8, 0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>F:(2, 97)37.2, 0</t>
+          <t>F:(2, 132)43.9, 0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>F:(3, 126)78.5, 0</t>
+          <t>F:(3, 193)157.2, 0</t>
         </is>
       </c>
     </row>
@@ -431,17 +431,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>F:(4, 47)8.1, 0</t>
+          <t>F:(4, 47)10.2, 0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>F:(4, 47)2.8, 0.0365</t>
+          <t>F:(4, 47)1.1, 0.3644</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>F:(4, 46)2.3, 0.0766</t>
+          <t>F:(4, 46)2.4, 0.0605</t>
         </is>
       </c>
     </row>
@@ -453,17 +453,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F:(8, 114)5.2, 0</t>
+          <t>F:(8, 132)10.1, 0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F:(8, 97)2.4, 0.0217</t>
+          <t>F:(8, 132)2.4, 0.0174</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F:(12, 126)3, 9e-04</t>
+          <t>F:(12, 193)2.2, 0.0123</t>
         </is>
       </c>
     </row>

</xml_diff>